<commit_message>
cleanup of broken projects
</commit_message>
<xml_diff>
--- a/IoT-recon.xlsx
+++ b/IoT-recon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adam\Documents\Vivado_Projects\IoT-Recon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5FEE50-CB6D-4F4B-A187-AB0EF26D47D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310F67FE-6309-4258-9EF8-BE0B0EE220F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="5820" windowWidth="24285" windowHeight="15885" xr2:uid="{48D670A6-BDBD-444B-9E90-AD8629F39DC6}"/>
+    <workbookView xWindow="0" yWindow="5715" windowWidth="24285" windowHeight="15885" xr2:uid="{48D670A6-BDBD-444B-9E90-AD8629F39DC6}"/>
   </bookViews>
   <sheets>
     <sheet name="specs" sheetId="1" r:id="rId1"/>
@@ -208,7 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -223,13 +223,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -549,7 +551,7 @@
   <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,24 +567,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="E1" s="10" t="s">
+      <c r="B1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
     </row>
     <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -610,22 +612,22 @@
       <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="E4" s="10" t="s">
+      <c r="B4" s="15"/>
+      <c r="E4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="J4" s="10" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="J4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
       <c r="O4" s="7" t="s">
         <v>38</v>
       </c>
@@ -634,9 +636,6 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
-        <v>5568785</v>
-      </c>
       <c r="K5" s="1" t="s">
         <v>33</v>
       </c>
@@ -658,9 +657,6 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>5568785</v>
-      </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
@@ -672,293 +668,216 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7">
-        <v>5568785</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="4">
-        <v>31001</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="F7" s="10">
+        <v>27737</v>
+      </c>
+      <c r="G7" s="10">
         <v>70560</v>
       </c>
-      <c r="H7" s="4">
-        <v>43.935657999999997</v>
+      <c r="H7" s="10">
+        <v>39.309806999999999</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K7">
-        <v>31220</v>
-      </c>
-      <c r="L7" s="4">
-        <v>70560</v>
-      </c>
-      <c r="M7" s="8">
+      <c r="L7" s="4"/>
+      <c r="M7" s="8" t="e">
         <f>K7/L7</f>
-        <v>0.44246031746031744</v>
-      </c>
-      <c r="O7">
-        <v>28191</v>
-      </c>
-      <c r="P7" s="13">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="12" t="e">
         <f>O7/K7</f>
-        <v>0.90297885970531711</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8">
-        <v>5568785</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="4">
-        <v>1412</v>
-      </c>
-      <c r="G8" s="4">
+      <c r="F8" s="10">
+        <v>1525</v>
+      </c>
+      <c r="G8" s="10">
         <v>28800</v>
       </c>
-      <c r="H8" s="4">
-        <v>4.9027776999999997</v>
+      <c r="H8" s="10">
+        <v>5.2951389999999998</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K8">
-        <v>1426</v>
-      </c>
-      <c r="L8" s="4">
-        <v>28800</v>
-      </c>
-      <c r="M8" s="8">
+      <c r="L8" s="4"/>
+      <c r="M8" s="8" t="e">
         <f t="shared" ref="M8:M16" si="0">K8/L8</f>
-        <v>4.9513888888888892E-2</v>
-      </c>
-      <c r="O8">
-        <v>1009</v>
-      </c>
-      <c r="P8" s="13">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" s="12" t="e">
         <f t="shared" ref="P8:P49" si="1">O8/K8</f>
-        <v>0.70757363253856942</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
-        <v>5568785</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="4">
-        <v>41182</v>
-      </c>
-      <c r="G9" s="4">
+      <c r="F9" s="10">
+        <v>40526</v>
+      </c>
+      <c r="G9" s="10">
         <v>141120</v>
       </c>
-      <c r="H9" s="4">
-        <v>29.182255000000001</v>
+      <c r="H9" s="10">
+        <v>28.717404999999999</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K9">
-        <v>41360</v>
-      </c>
-      <c r="L9" s="4">
-        <v>141120</v>
-      </c>
-      <c r="M9" s="8">
+      <c r="L9" s="4"/>
+      <c r="M9" s="8" t="e">
         <f t="shared" si="0"/>
-        <v>0.29308390022675734</v>
-      </c>
-      <c r="O9">
-        <v>37587</v>
-      </c>
-      <c r="P9" s="13">
-        <f t="shared" si="1"/>
-        <v>0.90877659574468084</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="10">
         <v>124</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="10">
         <v>216</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="10">
         <v>57.407409999999999</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K10">
-        <v>124</v>
-      </c>
-      <c r="L10" s="4">
-        <v>216</v>
-      </c>
-      <c r="M10" s="8">
+      <c r="L10" s="4"/>
+      <c r="M10" s="8" t="e">
         <f t="shared" si="0"/>
-        <v>0.57407407407407407</v>
-      </c>
-      <c r="O10">
-        <v>124</v>
-      </c>
-      <c r="P10" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P10" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="E11" s="5" t="s">
+      <c r="B11" s="15"/>
+      <c r="E11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="10">
         <v>24</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="10">
         <v>360</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="10">
         <v>6.6666670000000003</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K11">
-        <v>24</v>
-      </c>
-      <c r="L11" s="4">
-        <v>360</v>
-      </c>
-      <c r="M11" s="8">
+      <c r="L11" s="4"/>
+      <c r="M11" s="8" t="e">
         <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="O11">
-        <v>24</v>
-      </c>
-      <c r="P11" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P11" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
-        <v>5568785</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="10">
         <v>10</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="10">
         <v>82</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="10">
         <v>12.195122</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K12">
-        <v>10</v>
-      </c>
-      <c r="L12" s="4">
-        <v>82</v>
-      </c>
-      <c r="M12" s="8">
+      <c r="L12" s="4"/>
+      <c r="M12" s="8" t="e">
         <f t="shared" si="0"/>
-        <v>0.12195121951219512</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P12" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13">
-        <v>5755758</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="10">
         <v>1</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="10">
         <v>196</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="10">
         <v>0.51020410000000005</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13" s="4">
-        <v>196</v>
-      </c>
-      <c r="M13" s="8">
+      <c r="L13" s="4"/>
+      <c r="M13" s="8" t="e">
         <f t="shared" si="0"/>
-        <v>5.1020408163265302E-3</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P13" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
-      </c>
-      <c r="B14">
-        <v>5755758</v>
       </c>
       <c r="E14" s="4"/>
       <c r="G14"/>
       <c r="H14"/>
       <c r="J14" s="4"/>
-      <c r="P14" s="13"/>
+      <c r="P14" s="12"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
-      </c>
-      <c r="B15">
-        <v>5755758</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>2</v>
@@ -968,579 +887,468 @@
       <c r="J15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P15" s="13"/>
+      <c r="P15" s="12"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B16">
-        <v>5755758</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="4">
-        <v>45779</v>
-      </c>
-      <c r="G16" s="4">
+      <c r="F16" s="10">
+        <v>41543</v>
+      </c>
+      <c r="G16" s="10">
         <v>70560</v>
       </c>
-      <c r="H16" s="4">
-        <v>64.879540000000006</v>
+      <c r="H16" s="10">
+        <v>58.876133000000003</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="4">
-        <v>46022</v>
-      </c>
-      <c r="L16" s="4">
-        <v>70560</v>
-      </c>
-      <c r="M16" s="8">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="8" t="e">
         <f t="shared" si="0"/>
-        <v>0.65223922902494336</v>
-      </c>
-      <c r="O16">
-        <v>42993</v>
-      </c>
-      <c r="P16" s="13">
-        <f t="shared" si="1"/>
-        <v>0.93418365129720571</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P16" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B17">
-        <v>5755758</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="4">
-        <v>2308</v>
-      </c>
-      <c r="G17" s="4">
+      <c r="F17" s="10">
+        <v>2427</v>
+      </c>
+      <c r="G17" s="10">
         <v>28800</v>
       </c>
-      <c r="H17" s="4">
-        <v>8.0138890000000007</v>
+      <c r="H17" s="10">
+        <v>8.4270840000000007</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="4">
-        <v>2322</v>
-      </c>
-      <c r="L17" s="4">
-        <v>28800</v>
-      </c>
-      <c r="M17" s="8">
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="8" t="e">
         <f>K17/L17</f>
-        <v>8.0625000000000002E-2</v>
-      </c>
-      <c r="O17">
-        <v>1905</v>
-      </c>
-      <c r="P17" s="13">
-        <f t="shared" si="1"/>
-        <v>0.82041343669250644</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="4">
-        <v>53405</v>
-      </c>
-      <c r="G18" s="4">
+      <c r="F18" s="10">
+        <v>50740</v>
+      </c>
+      <c r="G18" s="10">
         <v>141120</v>
       </c>
-      <c r="H18" s="4">
-        <v>37.843679999999999</v>
+      <c r="H18" s="10">
+        <v>35.955215000000003</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="4">
-        <v>53620</v>
-      </c>
-      <c r="L18" s="4">
-        <v>141120</v>
-      </c>
-      <c r="M18" s="8">
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="8" t="e">
         <f t="shared" ref="M18:M49" si="2">K18/L18</f>
-        <v>0.37996031746031744</v>
-      </c>
-      <c r="O18">
-        <v>49847</v>
-      </c>
-      <c r="P18" s="13">
-        <f t="shared" si="1"/>
-        <v>0.92963446475195821</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P18" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="5" t="s">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="10">
         <v>131.5</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="10">
         <v>216</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="10">
         <v>60.879629999999999</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K19" s="4">
-        <v>131.5</v>
-      </c>
-      <c r="L19" s="4">
-        <v>216</v>
-      </c>
-      <c r="M19" s="8">
-        <f t="shared" si="2"/>
-        <v>0.60879629629629628</v>
-      </c>
-      <c r="O19">
-        <v>131.5</v>
-      </c>
-      <c r="P19" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P19" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="5" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="10">
         <v>26</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="10">
         <v>360</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="10">
         <v>7.2222223000000003</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K20" s="4">
-        <v>26</v>
-      </c>
-      <c r="L20" s="4">
-        <v>360</v>
-      </c>
-      <c r="M20" s="8">
-        <f t="shared" si="2"/>
-        <v>7.2222222222222215E-2</v>
-      </c>
-      <c r="O20">
-        <v>26</v>
-      </c>
-      <c r="P20" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P20" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="5" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="10">
         <v>10</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="10">
         <v>82</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="10">
         <v>12.195122</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K21" s="4">
-        <v>10</v>
-      </c>
-      <c r="L21" s="4">
-        <v>82</v>
-      </c>
-      <c r="M21" s="8">
-        <f t="shared" si="2"/>
-        <v>0.12195121951219512</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="4" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="10">
         <v>1</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="10">
         <v>196</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="10">
         <v>0.51020410000000005</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="4">
-        <v>1</v>
-      </c>
-      <c r="L22" s="4">
-        <v>196</v>
-      </c>
-      <c r="M22" s="8">
-        <f t="shared" si="2"/>
-        <v>5.1020408163265302E-3</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P22" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="P23" s="13"/>
+      <c r="P23" s="12"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="P24" s="13"/>
+      <c r="P24" s="12"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="5" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="4">
-        <v>39556</v>
-      </c>
-      <c r="G25" s="4">
+      <c r="F25" s="10">
+        <v>36200</v>
+      </c>
+      <c r="G25" s="10">
         <v>70560</v>
       </c>
-      <c r="H25" s="4">
-        <v>56.060093000000002</v>
+      <c r="H25" s="10">
+        <v>51.303856000000003</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K25">
-        <v>39779</v>
-      </c>
-      <c r="L25" s="4">
-        <v>70560</v>
-      </c>
-      <c r="M25" s="8">
-        <f t="shared" si="2"/>
-        <v>0.56376133786848071</v>
-      </c>
-      <c r="O25">
-        <v>36750</v>
-      </c>
-      <c r="P25" s="13">
-        <f t="shared" si="1"/>
-        <v>0.92385429497976324</v>
+      <c r="L25" s="4"/>
+      <c r="M25" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P25" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="4" t="s">
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="4">
-        <v>3716</v>
-      </c>
-      <c r="G26" s="4">
+      <c r="F26" s="10">
+        <v>3830</v>
+      </c>
+      <c r="G26" s="10">
         <v>28800</v>
       </c>
-      <c r="H26" s="4">
-        <v>12.902779000000001</v>
+      <c r="H26" s="10">
+        <v>13.298612</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K26">
-        <v>3730</v>
-      </c>
-      <c r="L26" s="4">
-        <v>28800</v>
-      </c>
-      <c r="M26" s="8">
-        <f t="shared" si="2"/>
-        <v>0.1295138888888889</v>
-      </c>
-      <c r="O26">
-        <v>3313</v>
-      </c>
-      <c r="P26" s="13">
-        <f t="shared" si="1"/>
-        <v>0.88820375335120638</v>
+      <c r="L26" s="4"/>
+      <c r="M26" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P26" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="4" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="4">
-        <v>49811</v>
-      </c>
-      <c r="G27" s="4">
+      <c r="F27" s="10">
+        <v>47792</v>
+      </c>
+      <c r="G27" s="10">
         <v>141120</v>
       </c>
-      <c r="H27" s="4">
-        <v>35.296909999999997</v>
+      <c r="H27" s="10">
+        <v>33.866210000000002</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K27">
-        <v>50064</v>
-      </c>
-      <c r="L27" s="4">
-        <v>141120</v>
-      </c>
-      <c r="M27" s="8">
-        <f t="shared" si="2"/>
-        <v>0.35476190476190478</v>
-      </c>
-      <c r="O27">
-        <v>46291</v>
-      </c>
-      <c r="P27" s="13">
-        <f t="shared" si="1"/>
-        <v>0.92463646532438482</v>
+      <c r="L27" s="4"/>
+      <c r="M27" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P27" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="4" t="s">
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="10">
         <v>154.5</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="10">
         <v>216</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="10">
         <v>71.527780000000007</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K28">
-        <v>154.5</v>
-      </c>
-      <c r="L28" s="4">
-        <v>216</v>
-      </c>
-      <c r="M28" s="8">
-        <f t="shared" si="2"/>
-        <v>0.71527777777777779</v>
-      </c>
-      <c r="O28">
-        <v>154.5</v>
-      </c>
-      <c r="P28" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="L28" s="4"/>
+      <c r="M28" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P28" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="4" t="s">
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="10">
         <v>32</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="10">
         <v>360</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="10">
         <v>8.8888890000000007</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K29">
-        <v>32</v>
-      </c>
-      <c r="L29" s="4">
-        <v>360</v>
-      </c>
-      <c r="M29" s="8">
-        <f t="shared" si="2"/>
-        <v>8.8888888888888892E-2</v>
-      </c>
-      <c r="O29">
-        <v>32</v>
-      </c>
-      <c r="P29" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="L29" s="4"/>
+      <c r="M29" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P29" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="10">
         <v>10</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="10">
         <v>82</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="10">
         <v>12.195122</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K30">
-        <v>10</v>
-      </c>
-      <c r="L30" s="4">
-        <v>82</v>
-      </c>
-      <c r="M30" s="8">
-        <f t="shared" si="2"/>
-        <v>0.12195121951219512</v>
-      </c>
-      <c r="O30">
-        <v>0</v>
-      </c>
-      <c r="P30" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="L30" s="4"/>
+      <c r="M30" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P30" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="10">
         <v>1</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="10">
         <v>196</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H31" s="10">
         <v>0.51020410000000005</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-      <c r="L31" s="4">
-        <v>196</v>
-      </c>
-      <c r="M31" s="8">
-        <f t="shared" si="2"/>
-        <v>5.1020408163265302E-3</v>
-      </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
-      <c r="P31" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="L31" s="4"/>
+      <c r="M31" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P31" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J32" s="4"/>
-      <c r="P32" s="13"/>
+      <c r="P32" s="12"/>
     </row>
     <row r="33" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E33" s="1" t="s">
@@ -1549,249 +1357,193 @@
       <c r="J33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P33" s="13"/>
+      <c r="P33" s="12"/>
     </row>
     <row r="34" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="4">
-        <v>27231</v>
-      </c>
-      <c r="G34" s="4">
+      <c r="F34" s="10">
+        <v>26809</v>
+      </c>
+      <c r="G34" s="10">
         <v>70560</v>
       </c>
-      <c r="H34" s="4">
-        <v>38.592686</v>
+      <c r="H34" s="10">
+        <v>37.994613999999999</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K34">
-        <v>31933</v>
-      </c>
-      <c r="L34" s="4">
-        <v>70560</v>
-      </c>
-      <c r="M34" s="8">
-        <f t="shared" si="2"/>
-        <v>0.45256519274376417</v>
-      </c>
-      <c r="O34">
-        <v>28904</v>
-      </c>
-      <c r="P34" s="13">
-        <f t="shared" si="1"/>
-        <v>0.90514514765289822</v>
+      <c r="L34" s="4"/>
+      <c r="M34" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P34" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="10">
         <v>1731</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="10">
         <v>28800</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35" s="10">
         <v>6.0104164999999998</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K35">
-        <v>1743</v>
-      </c>
-      <c r="L35" s="4">
-        <v>28800</v>
-      </c>
-      <c r="M35" s="8">
-        <f t="shared" si="2"/>
-        <v>6.0520833333333336E-2</v>
-      </c>
-      <c r="O35">
-        <v>1326</v>
-      </c>
-      <c r="P35" s="13">
-        <f t="shared" si="1"/>
-        <v>0.76075731497418242</v>
+      <c r="L35" s="4"/>
+      <c r="M35" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P35" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="4">
-        <v>30960</v>
-      </c>
-      <c r="G36" s="4">
+      <c r="F36" s="10">
+        <v>30951</v>
+      </c>
+      <c r="G36" s="10">
         <v>141120</v>
       </c>
-      <c r="H36" s="4">
-        <v>21.938776000000001</v>
+      <c r="H36" s="10">
+        <v>21.932397999999999</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K36">
-        <v>31193</v>
-      </c>
-      <c r="L36" s="4">
-        <v>141120</v>
-      </c>
-      <c r="M36" s="8">
-        <f t="shared" si="2"/>
-        <v>0.22103883219954648</v>
-      </c>
-      <c r="O36">
-        <v>27420</v>
-      </c>
-      <c r="P36" s="13">
-        <f t="shared" si="1"/>
-        <v>0.879043375116212</v>
+      <c r="L36" s="4"/>
+      <c r="M36" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P36" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="10">
         <v>110</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="10">
         <v>216</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="10">
         <v>50.925930000000001</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K37">
-        <v>110</v>
-      </c>
-      <c r="L37" s="4">
-        <v>216</v>
-      </c>
-      <c r="M37" s="8">
-        <f t="shared" si="2"/>
-        <v>0.5092592592592593</v>
-      </c>
-      <c r="O37">
-        <v>110</v>
-      </c>
-      <c r="P37" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="L37" s="4"/>
+      <c r="M37" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P37" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="38" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="10">
         <v>4</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="10">
         <v>360</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="10">
         <v>1.1111112000000001</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K38">
-        <v>4</v>
-      </c>
-      <c r="L38" s="4">
-        <v>360</v>
-      </c>
-      <c r="M38" s="8">
-        <f t="shared" si="2"/>
-        <v>1.1111111111111112E-2</v>
-      </c>
-      <c r="O38">
-        <v>4</v>
-      </c>
-      <c r="P38" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="L38" s="4"/>
+      <c r="M38" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P38" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="39" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="10">
         <v>10</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="10">
         <v>82</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39" s="10">
         <v>12.195122</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K39">
-        <v>10</v>
-      </c>
-      <c r="L39" s="4">
-        <v>82</v>
-      </c>
-      <c r="M39" s="8">
-        <f t="shared" si="2"/>
-        <v>0.12195121951219512</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="L39" s="4"/>
+      <c r="M39" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P39" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="40" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F40" s="10">
         <v>1</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="10">
         <v>196</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="10">
         <v>0.51020410000000005</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K40">
-        <v>1</v>
-      </c>
-      <c r="L40" s="4">
-        <v>196</v>
-      </c>
-      <c r="M40" s="8">
-        <f t="shared" si="2"/>
-        <v>5.1020408163265302E-3</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="L40" s="4"/>
+      <c r="M40" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P40" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="41" spans="5:16" x14ac:dyDescent="0.25">
       <c r="J41" s="4"/>
-      <c r="P41" s="13"/>
+      <c r="P41" s="12"/>
     </row>
     <row r="42" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E42" s="1" t="s">
@@ -1800,265 +1552,209 @@
       <c r="J42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P42" s="13"/>
+      <c r="P42" s="12"/>
     </row>
     <row r="43" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F43" s="4">
-        <v>48086</v>
-      </c>
-      <c r="G43" s="4">
+      <c r="F43" s="10">
+        <v>47695</v>
+      </c>
+      <c r="G43" s="10">
         <v>70560</v>
       </c>
-      <c r="H43" s="4">
-        <v>68.149090000000001</v>
+      <c r="H43" s="10">
+        <v>67.594954999999999</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K43">
-        <v>53433</v>
-      </c>
-      <c r="L43" s="4">
-        <v>70560</v>
-      </c>
-      <c r="M43" s="8">
-        <f t="shared" si="2"/>
-        <v>0.7572704081632653</v>
-      </c>
-      <c r="O43">
-        <v>50404</v>
-      </c>
-      <c r="P43" s="13">
-        <f t="shared" si="1"/>
-        <v>0.94331218535362038</v>
+      <c r="L43" s="4"/>
+      <c r="M43" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P43" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="44" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44" s="10">
         <v>2822</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="10">
         <v>28800</v>
       </c>
-      <c r="H44" s="4">
+      <c r="H44" s="10">
         <v>9.7986109999999993</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K44">
-        <v>2831</v>
-      </c>
-      <c r="L44" s="4">
-        <v>28800</v>
-      </c>
-      <c r="M44" s="8">
-        <f t="shared" si="2"/>
-        <v>9.8298611111111114E-2</v>
-      </c>
-      <c r="O44">
-        <v>2414</v>
-      </c>
-      <c r="P44" s="13">
-        <f t="shared" si="1"/>
-        <v>0.85270222536206286</v>
+      <c r="L44" s="4"/>
+      <c r="M44" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P44" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="45" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F45" s="4">
-        <v>35536</v>
-      </c>
-      <c r="G45" s="4">
+      <c r="F45" s="10">
+        <v>35521</v>
+      </c>
+      <c r="G45" s="10">
         <v>141120</v>
       </c>
-      <c r="H45" s="4">
-        <v>25.181405999999999</v>
+      <c r="H45" s="10">
+        <v>25.170776</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K45">
-        <v>39857</v>
-      </c>
-      <c r="L45" s="4">
-        <v>141120</v>
-      </c>
-      <c r="M45" s="8">
-        <f t="shared" si="2"/>
-        <v>0.28243339002267576</v>
-      </c>
-      <c r="O45">
-        <v>36084</v>
-      </c>
-      <c r="P45" s="13">
-        <f t="shared" si="1"/>
-        <v>0.90533657826730563</v>
+      <c r="L45" s="4"/>
+      <c r="M45" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P45" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="46" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F46" s="4">
+      <c r="F46" s="10">
         <v>110</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46" s="10">
         <v>216</v>
       </c>
-      <c r="H46" s="4">
+      <c r="H46" s="10">
         <v>50.925930000000001</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K46">
-        <v>110</v>
-      </c>
-      <c r="L46" s="4">
-        <v>216</v>
-      </c>
-      <c r="M46" s="8">
-        <f t="shared" si="2"/>
-        <v>0.5092592592592593</v>
-      </c>
-      <c r="O46">
-        <v>110</v>
-      </c>
-      <c r="P46" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="L46" s="4"/>
+      <c r="M46" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P46" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="47" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F47" s="10">
         <v>4</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="10">
         <v>360</v>
       </c>
-      <c r="H47" s="4">
+      <c r="H47" s="10">
         <v>1.1111112000000001</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K47">
-        <v>4</v>
-      </c>
-      <c r="L47" s="4">
-        <v>360</v>
-      </c>
-      <c r="M47" s="8">
-        <f t="shared" si="2"/>
-        <v>1.1111111111111112E-2</v>
-      </c>
-      <c r="O47">
-        <v>4</v>
-      </c>
-      <c r="P47" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="L47" s="4"/>
+      <c r="M47" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P47" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="48" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F48" s="10">
         <v>10</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48" s="10">
         <v>82</v>
       </c>
-      <c r="H48" s="4">
+      <c r="H48" s="10">
         <v>12.195122</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K48">
-        <v>10</v>
-      </c>
-      <c r="L48" s="4">
-        <v>82</v>
-      </c>
-      <c r="M48" s="8">
-        <f t="shared" si="2"/>
-        <v>0.12195121951219512</v>
-      </c>
-      <c r="O48">
-        <v>0</v>
-      </c>
-      <c r="P48" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="L48" s="4"/>
+      <c r="M48" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P48" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="49" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E49" s="4" t="s">
+      <c r="E49" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F49" s="4">
+      <c r="F49" s="10">
         <v>1</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G49" s="10">
         <v>196</v>
       </c>
-      <c r="H49" s="4">
+      <c r="H49" s="10">
         <v>0.51020410000000005</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K49">
-        <v>1</v>
-      </c>
-      <c r="L49" s="4">
-        <v>196</v>
-      </c>
-      <c r="M49" s="8">
-        <f t="shared" si="2"/>
-        <v>5.1020408163265302E-3</v>
-      </c>
-      <c r="O49">
-        <v>0</v>
-      </c>
-      <c r="P49" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="L49" s="4"/>
+      <c r="M49" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P49" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="E1:P1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="E1:P1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="E4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2087,10 +1783,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="15"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -2127,10 +1823,10 @@
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="15"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">

</xml_diff>

<commit_message>
rough workflow instructions and re-add full recon
</commit_message>
<xml_diff>
--- a/IoT-recon.xlsx
+++ b/IoT-recon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adam\Documents\Vivado_Projects\IoT-Recon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83637B75-5AA5-49EA-8261-4C19DE252D89}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60374A8B-0C0B-4664-8C24-76EB6F5A7E13}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="3465" windowWidth="24285" windowHeight="15885" xr2:uid="{48D670A6-BDBD-444B-9E90-AD8629F39DC6}"/>
+    <workbookView xWindow="-27045" yWindow="5250" windowWidth="24285" windowHeight="15885" xr2:uid="{48D670A6-BDBD-444B-9E90-AD8629F39DC6}"/>
   </bookViews>
   <sheets>
     <sheet name="specs" sheetId="1" r:id="rId1"/>
@@ -208,7 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -234,11 +234,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD2EDEE1-3369-479B-AE07-FACAD3ED1A6B}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,24 +574,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="E1" s="19" t="s">
+      <c r="B1" s="22"/>
+      <c r="E1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
     </row>
     <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -618,22 +619,22 @@
       <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="E4" s="19" t="s">
+      <c r="B4" s="22"/>
+      <c r="E4" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="J4" s="19" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="J4" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
       <c r="O4" s="7" t="s">
         <v>38</v>
       </c>
@@ -699,16 +700,22 @@
       <c r="J7" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="K7">
+        <v>31499</v>
+      </c>
       <c r="L7" s="17">
         <v>70560</v>
       </c>
       <c r="M7" s="8">
         <f>K7/L7</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="10" t="e">
+        <v>0.44641439909297054</v>
+      </c>
+      <c r="O7">
+        <v>28280</v>
+      </c>
+      <c r="P7" s="10">
         <f>O7/K7</f>
-        <v>#DIV/0!</v>
+        <v>0.8978062795644306</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -734,16 +741,22 @@
       <c r="J8" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="K8">
+        <v>1508</v>
+      </c>
       <c r="L8" s="17">
         <v>28800</v>
       </c>
       <c r="M8" s="8">
         <f t="shared" ref="M8:M16" si="0">K8/L8</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="10" t="e">
+        <v>5.2361111111111108E-2</v>
+      </c>
+      <c r="O8">
+        <v>1101</v>
+      </c>
+      <c r="P8" s="10">
         <f t="shared" ref="P8:P49" si="1">O8/K8</f>
-        <v>#DIV/0!</v>
+        <v>0.730106100795756</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -769,16 +782,22 @@
       <c r="J9" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="K9">
+        <v>41445</v>
+      </c>
       <c r="L9" s="17">
         <v>141120</v>
       </c>
       <c r="M9" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.29368622448979592</v>
+      </c>
+      <c r="O9">
+        <v>37587</v>
+      </c>
+      <c r="P9" s="10">
+        <f t="shared" si="1"/>
+        <v>0.90691277596815056</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -798,23 +817,29 @@
       <c r="J10" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="K10">
+        <v>124</v>
+      </c>
       <c r="L10" s="17">
         <v>216</v>
       </c>
       <c r="M10" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P10" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.57407407407407407</v>
+      </c>
+      <c r="O10">
+        <v>124</v>
+      </c>
+      <c r="P10" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="19"/>
+      <c r="B11" s="22"/>
       <c r="E11" s="14" t="s">
         <v>27</v>
       </c>
@@ -831,22 +856,31 @@
       <c r="J11" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="K11">
+        <v>24</v>
+      </c>
       <c r="L11" s="17">
         <v>360</v>
       </c>
       <c r="M11" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="O11">
+        <v>24</v>
+      </c>
+      <c r="P11" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="B12">
+        <v>5568785</v>
+      </c>
       <c r="E12" s="14" t="s">
         <v>30</v>
       </c>
@@ -863,21 +897,30 @@
       <c r="J12" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
       <c r="L12" s="17">
         <v>82</v>
       </c>
       <c r="M12" s="8">
         <f t="shared" si="0"/>
+        <v>0.12195121951219512</v>
+      </c>
+      <c r="O12">
         <v>0</v>
       </c>
-      <c r="P12" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="P12" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
+      </c>
+      <c r="B13">
+        <v>5746542</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>31</v>
@@ -895,21 +938,30 @@
       <c r="J13" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
       <c r="L13" s="17">
         <v>196</v>
       </c>
       <c r="M13" s="8">
         <f t="shared" si="0"/>
+        <v>5.1020408163265302E-3</v>
+      </c>
+      <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="P13" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
+      </c>
+      <c r="B14" s="19">
+        <v>5746542</v>
       </c>
       <c r="E14" s="4"/>
       <c r="G14"/>
@@ -922,6 +974,9 @@
       <c r="A15" t="s">
         <v>3</v>
       </c>
+      <c r="B15" s="19">
+        <v>5746542</v>
+      </c>
       <c r="E15" s="6" t="s">
         <v>2</v>
       </c>
@@ -937,6 +992,9 @@
       <c r="A16" t="s">
         <v>4</v>
       </c>
+      <c r="B16" s="19">
+        <v>5746542</v>
+      </c>
       <c r="E16" s="12" t="s">
         <v>25</v>
       </c>
@@ -952,23 +1010,31 @@
       <c r="J16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="4"/>
+      <c r="K16" s="4">
+        <v>46206</v>
+      </c>
       <c r="L16" s="17">
         <v>70560</v>
       </c>
       <c r="M16" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.65484693877551026</v>
+      </c>
+      <c r="O16">
+        <v>42987</v>
+      </c>
+      <c r="P16" s="10">
+        <f t="shared" si="1"/>
+        <v>0.93033372289313077</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
+      <c r="B17" s="19">
+        <v>5746542</v>
+      </c>
       <c r="E17" s="12" t="s">
         <v>28</v>
       </c>
@@ -984,17 +1050,22 @@
       <c r="J17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="4"/>
+      <c r="K17" s="4">
+        <v>2312</v>
+      </c>
       <c r="L17" s="17">
         <v>28800</v>
       </c>
       <c r="M17" s="8">
         <f>K17/L17</f>
-        <v>0</v>
-      </c>
-      <c r="P17" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>8.0277777777777781E-2</v>
+      </c>
+      <c r="O17">
+        <v>1905</v>
+      </c>
+      <c r="P17" s="10">
+        <f t="shared" si="1"/>
+        <v>0.82396193771626303</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1013,17 +1084,22 @@
       <c r="J18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="4"/>
+      <c r="K18" s="4">
+        <v>53673</v>
+      </c>
       <c r="L18" s="17">
         <v>141120</v>
       </c>
       <c r="M18" s="8">
         <f t="shared" ref="M18:M49" si="2">K18/L18</f>
-        <v>0</v>
-      </c>
-      <c r="P18" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.38033588435374149</v>
+      </c>
+      <c r="O18">
+        <v>49815</v>
+      </c>
+      <c r="P18" s="10">
+        <f t="shared" si="1"/>
+        <v>0.92812028394164658</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -1048,17 +1124,22 @@
       <c r="J19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K19" s="4"/>
+      <c r="K19" s="4">
+        <v>131.5</v>
+      </c>
       <c r="L19" s="17">
         <v>216</v>
       </c>
       <c r="M19" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.60879629629629628</v>
+      </c>
+      <c r="O19">
+        <v>131.5</v>
+      </c>
+      <c r="P19" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -1083,17 +1164,22 @@
       <c r="J20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K20" s="4"/>
+      <c r="K20" s="4">
+        <v>26</v>
+      </c>
       <c r="L20" s="17">
         <v>360</v>
       </c>
       <c r="M20" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>7.2222222222222215E-2</v>
+      </c>
+      <c r="O20">
+        <v>26</v>
+      </c>
+      <c r="P20" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1118,17 +1204,22 @@
       <c r="J21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K21" s="4"/>
+      <c r="K21" s="4">
+        <v>10</v>
+      </c>
       <c r="L21" s="17">
         <v>82</v>
       </c>
       <c r="M21" s="8">
         <f t="shared" si="2"/>
+        <v>0.12195121951219512</v>
+      </c>
+      <c r="O21">
         <v>0</v>
       </c>
-      <c r="P21" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="P21" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1153,17 +1244,22 @@
       <c r="J22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="4"/>
+      <c r="K22" s="4">
+        <v>1</v>
+      </c>
       <c r="L22" s="17">
         <v>196</v>
       </c>
       <c r="M22" s="8">
         <f t="shared" si="2"/>
+        <v>5.1020408163265302E-3</v>
+      </c>
+      <c r="O22">
         <v>0</v>
       </c>
-      <c r="P22" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="P22" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -1216,16 +1312,22 @@
       <c r="J25" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="K25">
+        <v>40079</v>
+      </c>
       <c r="L25" s="17">
         <v>70560</v>
       </c>
       <c r="M25" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.56801303854875285</v>
+      </c>
+      <c r="O25" s="19">
+        <v>36860</v>
+      </c>
+      <c r="P25" s="10">
+        <f>O25/K25</f>
+        <v>0.91968362484093913</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -1250,16 +1352,22 @@
       <c r="J26" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="K26">
+        <v>3811</v>
+      </c>
       <c r="L26" s="17">
         <v>28800</v>
       </c>
       <c r="M26" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P26" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.1323263888888889</v>
+      </c>
+      <c r="O26" s="19">
+        <v>3404</v>
+      </c>
+      <c r="P26" s="10">
+        <f>O26/K26</f>
+        <v>0.89320388349514568</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -1284,16 +1392,22 @@
       <c r="J27" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="K27">
+        <v>50075</v>
+      </c>
       <c r="L27" s="17">
         <v>141120</v>
       </c>
       <c r="M27" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P27" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.35483985260770973</v>
+      </c>
+      <c r="O27" s="19">
+        <v>46217</v>
+      </c>
+      <c r="P27" s="10">
+        <f>O27/K27</f>
+        <v>0.92295556665002498</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -1318,16 +1432,22 @@
       <c r="J28" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="K28">
+        <v>154.5</v>
+      </c>
       <c r="L28" s="17">
         <v>216</v>
       </c>
       <c r="M28" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P28" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="O28" s="19">
+        <v>154.5</v>
+      </c>
+      <c r="P28" s="10">
+        <f>O28/K28</f>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -1352,16 +1472,22 @@
       <c r="J29" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="K29">
+        <v>32</v>
+      </c>
       <c r="L29" s="17">
         <v>360</v>
       </c>
       <c r="M29" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P29" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="O29" s="19">
+        <v>32</v>
+      </c>
+      <c r="P29" s="10">
+        <f>O29/K29</f>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -1380,16 +1506,22 @@
       <c r="J30" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="K30">
+        <v>10</v>
+      </c>
       <c r="L30" s="17">
         <v>82</v>
       </c>
       <c r="M30" s="8">
         <f t="shared" si="2"/>
+        <v>0.12195121951219512</v>
+      </c>
+      <c r="O30" s="19">
         <v>0</v>
       </c>
-      <c r="P30" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="P30" s="10">
+        <f>O30/K30</f>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -1408,16 +1540,22 @@
       <c r="J31" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
       <c r="L31" s="17">
         <v>196</v>
       </c>
       <c r="M31" s="8">
         <f t="shared" si="2"/>
+        <v>5.1020408163265302E-3</v>
+      </c>
+      <c r="O31" s="19">
         <v>0</v>
       </c>
-      <c r="P31" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="P31" s="10">
+        <f>O31/K31</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -1449,16 +1587,22 @@
       <c r="J34" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="K34">
+        <v>32253</v>
+      </c>
       <c r="L34" s="17">
         <v>70560</v>
       </c>
       <c r="M34" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P34" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.45710034013605444</v>
+      </c>
+      <c r="O34">
+        <v>29034</v>
+      </c>
+      <c r="P34" s="10">
+        <f t="shared" si="1"/>
+        <v>0.90019533066691471</v>
       </c>
     </row>
     <row r="35" spans="5:16" x14ac:dyDescent="0.25">
@@ -1477,16 +1621,22 @@
       <c r="J35" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="K35">
+        <v>1884</v>
+      </c>
       <c r="L35" s="17">
         <v>28800</v>
       </c>
       <c r="M35" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P35" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>6.5416666666666665E-2</v>
+      </c>
+      <c r="O35">
+        <v>1477</v>
+      </c>
+      <c r="P35" s="10">
+        <f t="shared" si="1"/>
+        <v>0.78397027600849256</v>
       </c>
     </row>
     <row r="36" spans="5:16" x14ac:dyDescent="0.25">
@@ -1505,16 +1655,22 @@
       <c r="J36" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="K36">
+        <v>31273</v>
+      </c>
       <c r="L36" s="17">
         <v>141120</v>
       </c>
       <c r="M36" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P36" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.22160572562358277</v>
+      </c>
+      <c r="O36">
+        <v>27415</v>
+      </c>
+      <c r="P36" s="10">
+        <f t="shared" si="1"/>
+        <v>0.87663479678956291</v>
       </c>
     </row>
     <row r="37" spans="5:16" x14ac:dyDescent="0.25">
@@ -1533,16 +1689,22 @@
       <c r="J37" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="K37">
+        <v>110</v>
+      </c>
       <c r="L37" s="17">
         <v>216</v>
       </c>
       <c r="M37" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P37" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.5092592592592593</v>
+      </c>
+      <c r="O37">
+        <v>110</v>
+      </c>
+      <c r="P37" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="5:16" x14ac:dyDescent="0.25">
@@ -1561,16 +1723,22 @@
       <c r="J38" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="K38">
+        <v>4</v>
+      </c>
       <c r="L38" s="17">
         <v>360</v>
       </c>
       <c r="M38" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P38" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="O38">
+        <v>4</v>
+      </c>
+      <c r="P38" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="5:16" x14ac:dyDescent="0.25">
@@ -1589,16 +1757,22 @@
       <c r="J39" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="K39">
+        <v>10</v>
+      </c>
       <c r="L39" s="17">
         <v>82</v>
       </c>
       <c r="M39" s="8">
         <f t="shared" si="2"/>
+        <v>0.12195121951219512</v>
+      </c>
+      <c r="O39">
         <v>0</v>
       </c>
-      <c r="P39" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="P39" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="5:16" x14ac:dyDescent="0.25">
@@ -1617,16 +1791,22 @@
       <c r="J40" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
       <c r="L40" s="17">
         <v>196</v>
       </c>
       <c r="M40" s="8">
         <f t="shared" si="2"/>
+        <v>5.1020408163265302E-3</v>
+      </c>
+      <c r="O40">
         <v>0</v>
       </c>
-      <c r="P40" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="P40" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="5:16" x14ac:dyDescent="0.25">
@@ -1660,16 +1840,22 @@
       <c r="J43" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="K43">
+        <v>53879</v>
+      </c>
       <c r="L43" s="17">
         <v>70560</v>
       </c>
       <c r="M43" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P43" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.76359126984126979</v>
+      </c>
+      <c r="O43">
+        <v>50660</v>
+      </c>
+      <c r="P43" s="10">
+        <f t="shared" si="1"/>
+        <v>0.94025501586889138</v>
       </c>
     </row>
     <row r="44" spans="5:16" x14ac:dyDescent="0.25">
@@ -1688,16 +1874,22 @@
       <c r="J44" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="K44">
+        <v>3036</v>
+      </c>
       <c r="L44" s="17">
         <v>28800</v>
       </c>
       <c r="M44" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P44" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.10541666666666667</v>
+      </c>
+      <c r="O44">
+        <v>2629</v>
+      </c>
+      <c r="P44" s="10">
+        <f t="shared" si="1"/>
+        <v>0.86594202898550721</v>
       </c>
     </row>
     <row r="45" spans="5:16" x14ac:dyDescent="0.25">
@@ -1716,16 +1908,22 @@
       <c r="J45" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="K45">
+        <v>39842</v>
+      </c>
       <c r="L45" s="17">
         <v>141120</v>
       </c>
       <c r="M45" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P45" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.28232709750566892</v>
+      </c>
+      <c r="O45">
+        <v>35984</v>
+      </c>
+      <c r="P45" s="10">
+        <f t="shared" si="1"/>
+        <v>0.90316751167110088</v>
       </c>
     </row>
     <row r="46" spans="5:16" x14ac:dyDescent="0.25">
@@ -1744,16 +1942,22 @@
       <c r="J46" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="K46">
+        <v>110</v>
+      </c>
       <c r="L46" s="17">
         <v>216</v>
       </c>
       <c r="M46" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P46" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.5092592592592593</v>
+      </c>
+      <c r="O46">
+        <v>110</v>
+      </c>
+      <c r="P46" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="5:16" x14ac:dyDescent="0.25">
@@ -1772,16 +1976,22 @@
       <c r="J47" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="K47">
+        <v>4</v>
+      </c>
       <c r="L47" s="17">
         <v>360</v>
       </c>
       <c r="M47" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P47" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="O47">
+        <v>4</v>
+      </c>
+      <c r="P47" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="5:16" x14ac:dyDescent="0.25">
@@ -1800,16 +2010,22 @@
       <c r="J48" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="K48">
+        <v>10</v>
+      </c>
       <c r="L48" s="17">
         <v>82</v>
       </c>
       <c r="M48" s="8">
         <f t="shared" si="2"/>
+        <v>0.12195121951219512</v>
+      </c>
+      <c r="O48">
         <v>0</v>
       </c>
-      <c r="P48" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="P48" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="5:16" x14ac:dyDescent="0.25">
@@ -1828,16 +2044,22 @@
       <c r="J49" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
       <c r="L49" s="17">
         <v>196</v>
       </c>
       <c r="M49" s="8">
         <f t="shared" si="2"/>
+        <v>5.1020408163265302E-3</v>
+      </c>
+      <c r="O49">
         <v>0</v>
       </c>
-      <c r="P49" s="10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="P49" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="5:16" x14ac:dyDescent="0.25">
@@ -1869,23 +2091,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="E1:P1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="E1:P1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="E4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1914,10 +2136,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="19"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1954,10 +2176,10 @@
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="22"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">

</xml_diff>